<commit_message>
feat: add elderly on tables
</commit_message>
<xml_diff>
--- a/tables/table_100k_rates_2011_2019.xlsx
+++ b/tables/table_100k_rates_2011_2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t xml:space="preserve">Analise</t>
   </si>
@@ -61,6 +61,12 @@
     <t xml:space="preserve">Admissions_70_up_Tx</t>
   </si>
   <si>
+    <t xml:space="preserve">Admissions_non_elderly_Tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admissions_elderly_Tx</t>
+  </si>
+  <si>
     <t xml:space="preserve">Admissions_uti_20_49_Tx</t>
   </si>
   <si>
@@ -73,6 +79,12 @@
     <t xml:space="preserve">Admissions_uti_70_up_Tx</t>
   </si>
   <si>
+    <t xml:space="preserve">Admissions_uti_non_elderly_Tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admissions_uti_elderly_Tx</t>
+  </si>
+  <si>
     <t xml:space="preserve">Admissions_non_uti_20_49_Tx</t>
   </si>
   <si>
@@ -85,6 +97,12 @@
     <t xml:space="preserve">Admissions_non_uti_70_up_Tx</t>
   </si>
   <si>
+    <t xml:space="preserve">Admissions_non_uti_non_elderly_Tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admissions_non_uti_elderly_Tx</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mortes_20_49_Tx</t>
   </si>
   <si>
@@ -95,6 +113,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mortes_70_up_Tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortes_non_elderly_Tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortes_elderly_Tx</t>
   </si>
 </sst>
 </file>
@@ -220,17 +244,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q34" activeCellId="0" sqref="Q34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="8.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="6.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.87"/>
@@ -673,44 +697,44 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>4</v>
+        <v>137</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>25</v>
+        <v>-35.7664233576642</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3" t="n">
-        <v>0.44680220889739</v>
+        <v>-5.96180384384076</v>
       </c>
       <c r="O10" s="3" t="n">
-        <v>-0.198588579995718</v>
+        <v>-6.05462369608801</v>
       </c>
       <c r="P10" s="3" t="n">
-        <v>1.09636657874952</v>
+        <v>-5.86889228378086</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -721,44 +745,44 @@
         <v>14</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>11</v>
+        <v>956</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>12</v>
+        <v>874</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>14</v>
+        <v>897</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13</v>
+        <v>858</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>11</v>
+        <v>857</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>13</v>
+        <v>815</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>12</v>
+        <v>864</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>13</v>
+        <v>816</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>13</v>
+        <v>801</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>18.1818181818182</v>
+        <v>-16.2133891213389</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3" t="n">
-        <v>0.733761481666551</v>
+        <v>-1.708736896394</v>
       </c>
       <c r="O11" s="3" t="n">
-        <v>-0.857841109297064</v>
+        <v>-1.86390833636665</v>
       </c>
       <c r="P11" s="3" t="n">
-        <v>2.35091524920232</v>
+        <v>-1.55332010147217</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,44 +793,44 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L12" s="3" t="n">
         <v>25</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="J12" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="L12" s="3" t="n">
-        <v>20.8333333333333</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3" t="n">
-        <v>1.65896580903502</v>
+        <v>0.44680220889739</v>
       </c>
       <c r="O12" s="3" t="n">
-        <v>0.0213522638573993</v>
+        <v>-0.198588579995718</v>
       </c>
       <c r="P12" s="3" t="n">
-        <v>3.32339141046509</v>
+        <v>1.09636657874952</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,44 +841,44 @@
         <v>16</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>13.6986301369863</v>
+        <v>18.1818181818182</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3" t="n">
-        <v>0.329897865184114</v>
+        <v>0.733761481666551</v>
       </c>
       <c r="O13" s="3" t="n">
-        <v>-0.824845980048339</v>
+        <v>-0.857841109297064</v>
       </c>
       <c r="P13" s="3" t="n">
-        <v>1.49808694638598</v>
+        <v>2.35091524920232</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,44 +889,44 @@
         <v>17</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>-39.8148148148148</v>
+        <v>20.8333333333333</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3" t="n">
-        <v>-7.04479410187217</v>
+        <v>1.65896580903502</v>
       </c>
       <c r="O14" s="3" t="n">
-        <v>-7.17424831351397</v>
+        <v>0.0213522638573993</v>
       </c>
       <c r="P14" s="3" t="n">
-        <v>-6.915159354198</v>
+        <v>3.32339141046509</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,44 +937,44 @@
         <v>18</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>236</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>222</v>
+        <v>79</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>219</v>
+        <v>88</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>195</v>
+        <v>89</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>183</v>
+        <v>85</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>187</v>
+        <v>81</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>169</v>
+        <v>84</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>167</v>
+        <v>78</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>160</v>
+        <v>83</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>-32.2033898305085</v>
+        <v>13.6986301369863</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3" t="n">
-        <v>-4.86589601972363</v>
+        <v>0.329897865184114</v>
       </c>
       <c r="O15" s="3" t="n">
-        <v>-5.24387184973968</v>
+        <v>-0.824845980048339</v>
       </c>
       <c r="P15" s="3" t="n">
-        <v>-4.48641246951189</v>
+        <v>1.49808694638598</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,44 +985,44 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>458</v>
+        <v>5</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>417</v>
+        <v>6</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>423</v>
+        <v>6</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>385</v>
+        <v>6</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>374</v>
+        <v>5</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>373</v>
+        <v>6</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>376</v>
+        <v>5</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>354</v>
+        <v>6</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>342</v>
+        <v>6</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>-25.3275109170306</v>
+        <v>20</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3" t="n">
-        <v>-3.16170476320503</v>
+        <v>0.579466365188464</v>
       </c>
       <c r="O16" s="3" t="n">
-        <v>-3.56906845866718</v>
+        <v>0.134307216505136</v>
       </c>
       <c r="P16" s="3" t="n">
-        <v>-2.75262019687989</v>
+        <v>1.02660452259684</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,44 +1033,44 @@
         <v>20</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>1488</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>1347</v>
+        <v>49</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>1380</v>
+        <v>54</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>1339</v>
+        <v>54</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>1357</v>
+        <v>52</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>1263</v>
+        <v>51</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>1369</v>
+        <v>52</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>1293</v>
+        <v>50</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>1268</v>
+        <v>53</v>
       </c>
       <c r="L17" s="3" t="n">
-        <v>-14.7849462365591</v>
+        <v>15.2173913043478</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3" t="n">
-        <v>-1.37777695043196</v>
+        <v>0.720134349002621</v>
       </c>
       <c r="O17" s="3" t="n">
-        <v>-1.65915201177586</v>
+        <v>0.0664979210692529</v>
       </c>
       <c r="P17" s="3" t="n">
-        <v>-1.09559681239039</v>
+        <v>1.37804034356217</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,44 +1081,44 @@
         <v>21</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="L18" s="3" t="n">
-        <v>-16.6666666666667</v>
+        <v>-39.8148148148148</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3" t="n">
-        <v>-2.55305686396825</v>
+        <v>-7.04479410187217</v>
       </c>
       <c r="O18" s="3" t="n">
-        <v>-3.11280515384035</v>
+        <v>-7.17424831351397</v>
       </c>
       <c r="P18" s="3" t="n">
-        <v>-1.99007472932945</v>
+        <v>-6.915159354198</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,44 +1129,44 @@
         <v>22</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>22</v>
+        <v>236</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>22</v>
+        <v>222</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>23</v>
+        <v>219</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>21</v>
+        <v>195</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>21</v>
+        <v>183</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>21</v>
+        <v>167</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="L19" s="3" t="n">
-        <v>-9.09090909090909</v>
+        <v>-32.2033898305085</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3" t="n">
-        <v>-1.23796303846008</v>
+        <v>-4.86589601972363</v>
       </c>
       <c r="O19" s="3" t="n">
-        <v>-2.419539279918</v>
+        <v>-5.24387184973968</v>
       </c>
       <c r="P19" s="3" t="n">
-        <v>-0.0420793997622071</v>
+        <v>-4.48641246951189</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1153,44 +1177,44 @@
         <v>23</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>54</v>
+        <v>458</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>54</v>
+        <v>417</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>58</v>
+        <v>423</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>54</v>
+        <v>385</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>55</v>
+        <v>374</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>58</v>
+        <v>373</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>55</v>
+        <v>376</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>55</v>
+        <v>354</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>56</v>
+        <v>342</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>3.7037037037037</v>
+        <v>-25.3275109170306</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3" t="n">
-        <v>0.205734875802155</v>
+        <v>-3.16170476320503</v>
       </c>
       <c r="O20" s="3" t="n">
-        <v>-0.911567581120121</v>
+        <v>-3.56906845866718</v>
       </c>
       <c r="P20" s="3" t="n">
-        <v>1.3356358242917</v>
+        <v>-2.75262019687989</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,44 +1225,1328 @@
         <v>24</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>277</v>
+        <v>1488</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>279</v>
+        <v>1347</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>293</v>
+        <v>1380</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>289</v>
+        <v>1339</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>299</v>
+        <v>1357</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>300</v>
+        <v>1263</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>301</v>
+        <v>1369</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>293</v>
+        <v>1293</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>293</v>
+        <v>1268</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>5.77617328519856</v>
+        <v>-14.7849462365591</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3" t="n">
+        <v>-1.37777695043196</v>
+      </c>
+      <c r="O21" s="3" t="n">
+        <v>-1.65915201177586</v>
+      </c>
+      <c r="P21" s="3" t="n">
+        <v>-1.09559681239039</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="L22" s="3" t="n">
+        <v>-37.1212121212121</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3" t="n">
+        <v>-6.29060484960947</v>
+      </c>
+      <c r="O22" s="3" t="n">
+        <v>-6.38552758556182</v>
+      </c>
+      <c r="P22" s="3" t="n">
+        <v>-6.19558586437462</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>911</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>826</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>844</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>805</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>806</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>764</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>812</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>767</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>749</v>
+      </c>
+      <c r="L23" s="3" t="n">
+        <v>-17.7826564215148</v>
+      </c>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3" t="n">
+        <v>-1.85976124914515</v>
+      </c>
+      <c r="O23" s="3" t="n">
+        <v>-2.0194761392233</v>
+      </c>
+      <c r="P23" s="3" t="n">
+        <v>-1.69978601297876</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L24" s="3" t="n">
+        <v>-16.6666666666667</v>
+      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3" t="n">
+        <v>-2.55305686396825</v>
+      </c>
+      <c r="O24" s="3" t="n">
+        <v>-3.11280515384035</v>
+      </c>
+      <c r="P24" s="3" t="n">
+        <v>-1.99007472932945</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="L25" s="3" t="n">
+        <v>-9.09090909090909</v>
+      </c>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3" t="n">
+        <v>-1.23796303846008</v>
+      </c>
+      <c r="O25" s="3" t="n">
+        <v>-2.419539279918</v>
+      </c>
+      <c r="P25" s="3" t="n">
+        <v>-0.0420793997622071</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="L26" s="3" t="n">
+        <v>3.7037037037037</v>
+      </c>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3" t="n">
+        <v>0.205734875802155</v>
+      </c>
+      <c r="O26" s="3" t="n">
+        <v>-0.911567581120121</v>
+      </c>
+      <c r="P26" s="3" t="n">
+        <v>1.3356358242917</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>277</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>279</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>293</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>289</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>299</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>301</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>293</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>293</v>
+      </c>
+      <c r="L27" s="3" t="n">
+        <v>5.77617328519856</v>
+      </c>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3" t="n">
         <v>0.701835862369293</v>
       </c>
-      <c r="O21" s="3" t="n">
+      <c r="O27" s="3" t="n">
         <v>0.0853720861094587</v>
       </c>
-      <c r="P21" s="3" t="n">
+      <c r="P27" s="3" t="n">
         <v>1.32209667289618</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>-11.1111111111111</v>
+      </c>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3" t="n">
+        <v>-1.89046883300875</v>
+      </c>
+      <c r="O28" s="3" t="n">
+        <v>-2.24971121354072</v>
+      </c>
+      <c r="P28" s="3" t="n">
+        <v>-1.52990619972284</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>153</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>161</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>162</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>165</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>163</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>5.26315789473684</v>
+      </c>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3" t="n">
+        <v>0.604819287016967</v>
+      </c>
+      <c r="O29" s="3" t="n">
+        <v>0.235585756058421</v>
+      </c>
+      <c r="P29" s="3" t="n">
+        <v>0.975412947707421</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="L31" s="3" t="n">
+        <v>15.3846153846154</v>
+      </c>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3" t="n">
+        <v>0.712796305352637</v>
+      </c>
+      <c r="O31" s="3" t="n">
+        <v>0.484567222814847</v>
+      </c>
+      <c r="P31" s="3" t="n">
+        <v>0.941543761164598</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>274</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>251</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>254</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>235</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>225</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>217</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>218</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>204</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>-25.5474452554744</v>
+      </c>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3" t="n">
+        <v>-3.49011114212245</v>
+      </c>
+      <c r="O32" s="3" t="n">
+        <v>-3.54316525891049</v>
+      </c>
+      <c r="P32" s="3" t="n">
+        <v>-3.43702784399837</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="L33" s="3" t="n">
+        <v>-38.3928571428572</v>
+      </c>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3" t="n">
+        <v>-6.72381925703277</v>
+      </c>
+      <c r="O33" s="3" t="n">
+        <v>-6.85072404970131</v>
+      </c>
+      <c r="P33" s="3" t="n">
+        <v>-6.59674157170095</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3" t="n">
+        <v>0.44680220889739</v>
+      </c>
+      <c r="O34" s="3" t="n">
+        <v>-0.198588579995718</v>
+      </c>
+      <c r="P34" s="3" t="n">
+        <v>1.09636657874952</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>101</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="K35" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>-39.8148148148148</v>
+      </c>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3" t="n">
+        <v>-7.04479410187217</v>
+      </c>
+      <c r="O35" s="3" t="n">
+        <v>-7.17424831351397</v>
+      </c>
+      <c r="P35" s="3" t="n">
+        <v>-6.915159354198</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>247</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>233</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>232</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>207</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>180</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>180</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>172</v>
+      </c>
+      <c r="L36" s="3" t="n">
+        <v>-30.3643724696356</v>
+      </c>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3" t="n">
+        <v>-4.54448955209449</v>
+      </c>
+      <c r="O36" s="3" t="n">
+        <v>-4.91233673017614</v>
+      </c>
+      <c r="P36" s="3" t="n">
+        <v>-4.17521935506623</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="I37" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="J37" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="K37" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L37" s="3" t="n">
+        <v>18.1818181818182</v>
+      </c>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3" t="n">
+        <v>0.733761481666551</v>
+      </c>
+      <c r="O37" s="3" t="n">
+        <v>-0.857841109297064</v>
+      </c>
+      <c r="P37" s="3" t="n">
+        <v>2.35091524920232</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>236</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>222</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>219</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>195</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>183</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>187</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>169</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <v>167</v>
+      </c>
+      <c r="K38" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="L38" s="3" t="n">
+        <v>-32.2033898305085</v>
+      </c>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3" t="n">
+        <v>-4.86589601972363</v>
+      </c>
+      <c r="O38" s="3" t="n">
+        <v>-5.24387184973968</v>
+      </c>
+      <c r="P38" s="3" t="n">
+        <v>-4.48641246951189</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>482</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>441</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>450</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>411</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>399</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="I39" s="2" t="n">
+        <v>402</v>
+      </c>
+      <c r="J39" s="2" t="n">
+        <v>381</v>
+      </c>
+      <c r="K39" s="2" t="n">
+        <v>370</v>
+      </c>
+      <c r="L39" s="3" t="n">
+        <v>-23.2365145228216</v>
+      </c>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3" t="n">
+        <v>-2.86211404487777</v>
+      </c>
+      <c r="O39" s="3" t="n">
+        <v>-3.25756740999551</v>
+      </c>
+      <c r="P39" s="3" t="n">
+        <v>-2.46504418780511</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="K40" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="L40" s="3" t="n">
+        <v>20.8333333333333</v>
+      </c>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3" t="n">
+        <v>1.65896580903502</v>
+      </c>
+      <c r="O40" s="3" t="n">
+        <v>0.0213522638573993</v>
+      </c>
+      <c r="P40" s="3" t="n">
+        <v>3.32339141046509</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>458</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>417</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>423</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>385</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>374</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>373</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>376</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>354</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="L41" s="3" t="n">
+        <v>-25.3275109170306</v>
+      </c>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3" t="n">
+        <v>-3.16170476320503</v>
+      </c>
+      <c r="O41" s="3" t="n">
+        <v>-3.56906845866718</v>
+      </c>
+      <c r="P41" s="3" t="n">
+        <v>-2.75262019687989</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>1561</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>1426</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>1467</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>1428</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>1441</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>1343</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>1453</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>1371</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <v>1350</v>
+      </c>
+      <c r="L42" s="3" t="n">
+        <v>-13.5169762972454</v>
+      </c>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3" t="n">
+        <v>-1.28034189288327</v>
+      </c>
+      <c r="O42" s="3" t="n">
+        <v>-1.55380097324507</v>
+      </c>
+      <c r="P42" s="3" t="n">
+        <v>-1.00612321114153</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <v>84</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="L43" s="3" t="n">
+        <v>13.6986301369863</v>
+      </c>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3" t="n">
+        <v>0.329897865184114</v>
+      </c>
+      <c r="O43" s="3" t="n">
+        <v>-0.824845980048339</v>
+      </c>
+      <c r="P43" s="3" t="n">
+        <v>1.49808694638598</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>1488</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>1347</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>1380</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>1339</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <v>1357</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>1263</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <v>1369</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>1293</v>
+      </c>
+      <c r="K44" s="2" t="n">
+        <v>1268</v>
+      </c>
+      <c r="L44" s="3" t="n">
+        <v>-14.7849462365591</v>
+      </c>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3" t="n">
+        <v>-1.37777695043196</v>
+      </c>
+      <c r="O44" s="3" t="n">
+        <v>-1.65915201177586</v>
+      </c>
+      <c r="P44" s="3" t="n">
+        <v>-1.09559681239039</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>129</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="J45" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="L45" s="3" t="n">
+        <v>-35.7664233576642</v>
+      </c>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3" t="n">
+        <v>-5.96180384384076</v>
+      </c>
+      <c r="O45" s="3" t="n">
+        <v>-6.05462369608801</v>
+      </c>
+      <c r="P45" s="3" t="n">
+        <v>-5.86889228378086</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I46" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="K46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3" t="n">
+        <v>0.579466365188464</v>
+      </c>
+      <c r="O46" s="3" t="n">
+        <v>0.134307216505136</v>
+      </c>
+      <c r="P46" s="3" t="n">
+        <v>1.02660452259684</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="F47" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="G47" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="I47" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="K47" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="L47" s="3" t="n">
+        <v>-37.1212121212121</v>
+      </c>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3" t="n">
+        <v>-6.29060484960947</v>
+      </c>
+      <c r="O47" s="3" t="n">
+        <v>-6.38552758556182</v>
+      </c>
+      <c r="P47" s="3" t="n">
+        <v>-6.19558586437462</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>956</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>874</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>897</v>
+      </c>
+      <c r="F48" s="2" t="n">
+        <v>858</v>
+      </c>
+      <c r="G48" s="2" t="n">
+        <v>857</v>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>815</v>
+      </c>
+      <c r="I48" s="2" t="n">
+        <v>864</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <v>816</v>
+      </c>
+      <c r="K48" s="2" t="n">
+        <v>801</v>
+      </c>
+      <c r="L48" s="3" t="n">
+        <v>-16.2133891213389</v>
+      </c>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3" t="n">
+        <v>-1.708736896394</v>
+      </c>
+      <c r="O48" s="3" t="n">
+        <v>-1.86390833636665</v>
+      </c>
+      <c r="P48" s="3" t="n">
+        <v>-1.55332010147217</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="F49" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="G49" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="I49" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="K49" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="L49" s="3" t="n">
+        <v>15.2173913043478</v>
+      </c>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3" t="n">
+        <v>0.720134349002621</v>
+      </c>
+      <c r="O49" s="3" t="n">
+        <v>0.0664979210692529</v>
+      </c>
+      <c r="P49" s="3" t="n">
+        <v>1.37804034356217</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>911</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>826</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>844</v>
+      </c>
+      <c r="F50" s="2" t="n">
+        <v>805</v>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>806</v>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>764</v>
+      </c>
+      <c r="I50" s="2" t="n">
+        <v>812</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <v>767</v>
+      </c>
+      <c r="K50" s="2" t="n">
+        <v>749</v>
+      </c>
+      <c r="L50" s="3" t="n">
+        <v>-17.7826564215148</v>
+      </c>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3" t="n">
+        <v>-1.85976124914515</v>
+      </c>
+      <c r="O50" s="3" t="n">
+        <v>-2.0194761392233</v>
+      </c>
+      <c r="P50" s="3" t="n">
+        <v>-1.69978601297876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>